<commit_message>
AV Enge de Sofwtare ...... 07Jun2024
</commit_message>
<xml_diff>
--- a/03 Assessments/NOTAS AV - Enegenharia de Sofwtare - 2024.1 Wyden UniRuy.xlsx
+++ b/03 Assessments/NOTAS AV - Enegenharia de Sofwtare - 2024.1 Wyden UniRuy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\11 WydenArea1EngenhariaDeSoftware\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8BBA41-0F63-426C-A3A6-B2FAE6E0F392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCF724E-C0AE-4B7A-89D5-0930208D0559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{413AB662-3705-4BE9-8AD4-FDF0F3F54212}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>AV</t>
   </si>
@@ -306,6 +306,12 @@
   </si>
   <si>
     <t>GitHub - Ar1an3/GerTarefa: Projeto Disciplina - PooJ</t>
+  </si>
+  <si>
+    <t>PPT</t>
+  </si>
+  <si>
+    <t>??? Postou como entregue , mas não tem nada</t>
   </si>
 </sst>
 </file>
@@ -591,9 +597,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -624,6 +627,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -960,42 +966,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2841AE5-15C3-4767-A901-0C645FE8FC21}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+    </row>
+    <row r="2" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>87</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1004,14 +1011,17 @@
       <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
@@ -1021,11 +1031,12 @@
       <c r="C3" s="11">
         <v>0.9</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>39</v>
       </c>
@@ -1035,11 +1046,12 @@
       <c r="C4" s="12">
         <v>0.9</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="25"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>41</v>
       </c>
@@ -1049,14 +1061,15 @@
       <c r="C5" s="12">
         <v>0.5</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="1">
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>43</v>
       </c>
@@ -1066,17 +1079,18 @@
       <c r="C6" s="12">
         <v>0</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="1">
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="1">
         <v>4</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>45</v>
       </c>
@@ -1086,11 +1100,12 @@
       <c r="C7" s="12">
         <v>0</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="25"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>47</v>
       </c>
@@ -1100,14 +1115,15 @@
       <c r="C8" s="12">
         <v>0.3</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="1">
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>6</v>
       </c>
@@ -1117,14 +1133,15 @@
       <c r="C9" s="12">
         <v>0.4</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="1">
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
@@ -1134,11 +1151,12 @@
       <c r="C10" s="12">
         <v>0.5</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="25"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>49</v>
       </c>
@@ -1148,14 +1166,15 @@
       <c r="C11" s="12">
         <v>0.5</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="1">
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>10</v>
       </c>
@@ -1165,14 +1184,15 @@
       <c r="C12" s="12">
         <v>0.3</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="1">
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>51</v>
       </c>
@@ -1182,11 +1202,12 @@
       <c r="C13" s="12">
         <v>0.9</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="25"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>53</v>
       </c>
@@ -1196,11 +1217,12 @@
       <c r="C14" s="12">
         <v>0.9</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="25"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
@@ -1210,11 +1232,12 @@
       <c r="C15" s="12">
         <v>0.9</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="25"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>55</v>
       </c>
@@ -1224,11 +1247,12 @@
       <c r="C16" s="12">
         <v>0</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="25"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="24"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>57</v>
       </c>
@@ -1238,11 +1262,12 @@
       <c r="C17" s="12">
         <v>0.9</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="25"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="24"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>14</v>
       </c>
@@ -1252,11 +1277,12 @@
       <c r="C18" s="12">
         <v>0.3</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="25"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="24"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>59</v>
       </c>
@@ -1266,11 +1292,12 @@
       <c r="C19" s="12">
         <v>0.4</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="25"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="24"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>16</v>
       </c>
@@ -1280,11 +1307,12 @@
       <c r="C20" s="12">
         <v>0.8</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="25"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="24"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>18</v>
       </c>
@@ -1294,11 +1322,12 @@
       <c r="C21" s="12">
         <v>0</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="25"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="24"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>61</v>
       </c>
@@ -1308,11 +1337,12 @@
       <c r="C22" s="12">
         <v>0.5</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="25"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="24"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>63</v>
       </c>
@@ -1322,11 +1352,12 @@
       <c r="C23" s="12">
         <v>0</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="25"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>20</v>
       </c>
@@ -1336,11 +1367,12 @@
       <c r="C24" s="12">
         <v>0.5</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="25"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>65</v>
       </c>
@@ -1350,11 +1382,12 @@
       <c r="C25" s="12">
         <v>0.9</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="25"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>67</v>
       </c>
@@ -1364,11 +1397,12 @@
       <c r="C26" s="12">
         <v>0.9</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="25"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="24"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>69</v>
       </c>
@@ -1378,11 +1412,12 @@
       <c r="C27" s="12">
         <v>0.9</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="25"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="24"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>22</v>
       </c>
@@ -1392,11 +1427,12 @@
       <c r="C28" s="12">
         <v>1</v>
       </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="25"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="24"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>24</v>
       </c>
@@ -1406,11 +1442,12 @@
       <c r="C29" s="12">
         <v>1</v>
       </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="25"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>71</v>
       </c>
@@ -1420,14 +1457,15 @@
       <c r="C30" s="12">
         <v>0.6</v>
       </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="1">
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>73</v>
       </c>
@@ -1437,11 +1475,12 @@
       <c r="C31" s="12">
         <v>0.6</v>
       </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="25"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="24"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>26</v>
       </c>
@@ -1451,11 +1490,12 @@
       <c r="C32" s="12">
         <v>0.4</v>
       </c>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="25"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="24"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>75</v>
       </c>
@@ -1465,11 +1505,15 @@
       <c r="C33" s="12">
         <v>0.8</v>
       </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="25"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="24"/>
+      <c r="I33" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>4</v>
       </c>
@@ -1479,11 +1523,12 @@
       <c r="C34" s="12">
         <v>0.3</v>
       </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="25"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="24"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>77</v>
       </c>
@@ -1493,11 +1538,12 @@
       <c r="C35" s="12">
         <v>1</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="25"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>79</v>
       </c>
@@ -1507,11 +1553,12 @@
       <c r="C36" s="12">
         <v>0</v>
       </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="25"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="24"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>81</v>
       </c>
@@ -1521,11 +1568,12 @@
       <c r="C37" s="12">
         <v>0.8</v>
       </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="25"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="24"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>83</v>
       </c>
@@ -1535,11 +1583,15 @@
       <c r="C38" s="12">
         <v>0</v>
       </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="25"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>85</v>
       </c>
@@ -1549,11 +1601,12 @@
       <c r="C39" s="12">
         <v>0.9</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="25"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="24"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>28</v>
       </c>
@@ -1563,11 +1616,12 @@
       <c r="C40" s="12">
         <v>1</v>
       </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="25"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="24"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>30</v>
       </c>
@@ -1577,38 +1631,40 @@
       <c r="C41" s="12">
         <v>0.8</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="25"/>
-    </row>
-    <row r="42" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="24"/>
+    </row>
+    <row r="42" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C42" s="13">
         <v>0.3</v>
       </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="29"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="17" t="s">
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="28"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B44" s="16" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G42">
     <sortCondition ref="B3:B42"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" display="https://github.com/Ar1an3/GerTarefa" xr:uid="{3CC27A7A-E5AC-4FE0-879D-E1267B5AFB88}"/>
+    <hyperlink ref="I6" r:id="rId1" display="https://github.com/Ar1an3/GerTarefa" xr:uid="{3CC27A7A-E5AC-4FE0-879D-E1267B5AFB88}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>

</xml_diff>

<commit_message>
AV Engen de Sofwtare ...... 07Jun2024
</commit_message>
<xml_diff>
--- a/03 Assessments/NOTAS AV - Enegenharia de Sofwtare - 2024.1 Wyden UniRuy.xlsx
+++ b/03 Assessments/NOTAS AV - Enegenharia de Sofwtare - 2024.1 Wyden UniRuy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\11 WydenArea1EngenhariaDeSoftware\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCF724E-C0AE-4B7A-89D5-0930208D0559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A1F703-2CF3-46DF-8D00-71FD76019738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{413AB662-3705-4BE9-8AD4-FDF0F3F54212}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>AV</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>??? Postou como entregue , mas não tem nada</t>
+  </si>
+  <si>
+    <t>https://github.com/MasaoLH/projetoengenhariadesoftware</t>
   </si>
 </sst>
 </file>
@@ -968,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2841AE5-15C3-4767-A901-0C645FE8FC21}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1252,7 +1255,7 @@
       <c r="F16" s="20"/>
       <c r="G16" s="24"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>57</v>
       </c>
@@ -1267,7 +1270,7 @@
       <c r="F17" s="20"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>14</v>
       </c>
@@ -1282,7 +1285,7 @@
       <c r="F18" s="20"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>59</v>
       </c>
@@ -1297,7 +1300,7 @@
       <c r="F19" s="20"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>16</v>
       </c>
@@ -1312,7 +1315,7 @@
       <c r="F20" s="20"/>
       <c r="G20" s="24"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>18</v>
       </c>
@@ -1327,7 +1330,7 @@
       <c r="F21" s="20"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>61</v>
       </c>
@@ -1342,7 +1345,7 @@
       <c r="F22" s="20"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>63</v>
       </c>
@@ -1357,7 +1360,7 @@
       <c r="F23" s="20"/>
       <c r="G23" s="24"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>20</v>
       </c>
@@ -1372,7 +1375,7 @@
       <c r="F24" s="20"/>
       <c r="G24" s="24"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>65</v>
       </c>
@@ -1387,7 +1390,7 @@
       <c r="F25" s="20"/>
       <c r="G25" s="24"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>67</v>
       </c>
@@ -1402,7 +1405,7 @@
       <c r="F26" s="20"/>
       <c r="G26" s="24"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>69</v>
       </c>
@@ -1417,7 +1420,7 @@
       <c r="F27" s="20"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>22</v>
       </c>
@@ -1432,7 +1435,7 @@
       <c r="F28" s="20"/>
       <c r="G28" s="24"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>24</v>
       </c>
@@ -1447,7 +1450,7 @@
       <c r="F29" s="20"/>
       <c r="G29" s="24"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>71</v>
       </c>
@@ -1464,8 +1467,11 @@
       <c r="H30" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>73</v>
       </c>
@@ -1480,7 +1486,7 @@
       <c r="F31" s="20"/>
       <c r="G31" s="24"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
AV Engen de Sofwtare ...... 08Jun2024
</commit_message>
<xml_diff>
--- a/03 Assessments/NOTAS AV - Enegenharia de Sofwtare - 2024.1 Wyden UniRuy.xlsx
+++ b/03 Assessments/NOTAS AV - Enegenharia de Sofwtare - 2024.1 Wyden UniRuy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\11 WydenArea1EngenhariaDeSoftware\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A1F703-2CF3-46DF-8D00-71FD76019738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBDA332-E10D-4A97-BED8-E1F20A0A0532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{413AB662-3705-4BE9-8AD4-FDF0F3F54212}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
   <si>
     <t>AV</t>
   </si>
@@ -305,9 +305,6 @@
     <t>SSA, 07 de junho de 2024</t>
   </si>
   <si>
-    <t>GitHub - Ar1an3/GerTarefa: Projeto Disciplina - PooJ</t>
-  </si>
-  <si>
     <t>PPT</t>
   </si>
   <si>
@@ -315,6 +312,45 @@
   </si>
   <si>
     <t>https://github.com/MasaoLH/projetoengenhariadesoftware</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>ppt pelo celular</t>
+  </si>
+  <si>
+    <t>não ppt</t>
+  </si>
+  <si>
+    <t>ppt +-</t>
+  </si>
+  <si>
+    <t>GitHub - Ar1an3/GerTarefa: Projeto Disciplina - PooJ; ppt +-</t>
+  </si>
+  <si>
+    <t>GitHub - deivomaciel/Trabalho-Eng.-de-Software</t>
+  </si>
+  <si>
+    <t>https://github.com/ruiRomer/EngenhariadeSoftware-Sistema_de_Biblioteca</t>
+  </si>
+  <si>
+    <t>https://github.com/softwareengineeringp/Projeto_Engenharia_Software</t>
+  </si>
+  <si>
+    <t>GitHub - Germinio-marcelo/Engenharia-de-software-hugo..</t>
+  </si>
+  <si>
+    <t>não</t>
+  </si>
+  <si>
+    <t>não ppt; apresentou proposta de sistema</t>
+  </si>
+  <si>
+    <t>não apresentou os artefatos; arq externa dos componentes do app</t>
+  </si>
+  <si>
+    <t>??? Dúvida; Apresentou ppt? Acgo que sim, hospedagem site</t>
   </si>
 </sst>
 </file>
@@ -361,12 +397,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="14">
@@ -562,7 +610,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -620,19 +668,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -971,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2841AE5-15C3-4767-A901-0C645FE8FC21}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -980,23 +1036,24 @@
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="69.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="73.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1015,7 +1072,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>2</v>
@@ -1034,10 +1091,25 @@
       <c r="C3" s="11">
         <v>0.9</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
+      <c r="D3" s="21">
+        <v>4.8</v>
+      </c>
+      <c r="E3" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="G3" s="31">
+        <f>D3+E3+F3</f>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="H3" s="1">
+        <v>7</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
@@ -1049,10 +1121,22 @@
       <c r="C4" s="12">
         <v>0.9</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="24"/>
+      <c r="D4" s="19">
+        <v>4.8</v>
+      </c>
+      <c r="E4" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="F4" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G4" s="32">
+        <f>D4+E4+F4</f>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="H4" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
@@ -1064,10 +1148,19 @@
       <c r="C5" s="12">
         <v>0.5</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="24"/>
+      <c r="D5" s="19">
+        <v>5.4</v>
+      </c>
+      <c r="E5" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="F5" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="32">
+        <f t="shared" ref="G5:G41" si="0">D5+E5+F5</f>
+        <v>9.4</v>
+      </c>
       <c r="H5" s="1">
         <v>5</v>
       </c>
@@ -1082,15 +1175,24 @@
       <c r="C6" s="12">
         <v>0</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="24"/>
+      <c r="D6" s="19">
+        <v>4.2</v>
+      </c>
+      <c r="E6" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="G6" s="32">
+        <f t="shared" si="0"/>
+        <v>7.2</v>
+      </c>
       <c r="H6" s="1">
         <v>4</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1103,10 +1205,22 @@
       <c r="C7" s="12">
         <v>0</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="24"/>
+      <c r="D7" s="19">
+        <v>6</v>
+      </c>
+      <c r="E7" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="F7" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="32">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+      <c r="H7" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
@@ -1118,12 +1232,24 @@
       <c r="C8" s="12">
         <v>0.3</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="24"/>
+      <c r="D8" s="19">
+        <v>6</v>
+      </c>
+      <c r="E8" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="G8" s="32">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
       <c r="H8" s="1">
         <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1136,10 +1262,19 @@
       <c r="C9" s="12">
         <v>0.4</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="24"/>
+      <c r="D9" s="19">
+        <v>3</v>
+      </c>
+      <c r="E9" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F9" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G9" s="32">
+        <f t="shared" si="0"/>
+        <v>6.7</v>
+      </c>
       <c r="H9" s="1">
         <v>5</v>
       </c>
@@ -1154,10 +1289,25 @@
       <c r="C10" s="12">
         <v>0.5</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="24"/>
+      <c r="D10" s="19">
+        <v>6</v>
+      </c>
+      <c r="E10" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="F10" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G10" s="32">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H10" s="1">
+        <v>8</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
@@ -1169,12 +1319,24 @@
       <c r="C11" s="12">
         <v>0.5</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="24"/>
+      <c r="D11" s="19">
+        <v>2.4</v>
+      </c>
+      <c r="E11" s="19">
+        <v>2</v>
+      </c>
+      <c r="F11" s="27">
+        <v>0</v>
+      </c>
+      <c r="G11" s="32">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
       <c r="H11" s="1">
         <v>2</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1187,12 +1349,24 @@
       <c r="C12" s="12">
         <v>0.3</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="24"/>
+      <c r="D12" s="19">
+        <v>5.4</v>
+      </c>
+      <c r="E12" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="27">
+        <v>0</v>
+      </c>
+      <c r="G12" s="32">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
       <c r="H12" s="1">
         <v>3</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1205,10 +1379,22 @@
       <c r="C13" s="12">
         <v>0.9</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="24"/>
+      <c r="D13" s="19">
+        <v>5.4</v>
+      </c>
+      <c r="E13" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="F13" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G13" s="32">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+      <c r="H13" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -1220,10 +1406,22 @@
       <c r="C14" s="12">
         <v>0.9</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="24"/>
+      <c r="D14" s="19">
+        <v>6</v>
+      </c>
+      <c r="E14" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="27">
+        <v>0</v>
+      </c>
+      <c r="G14" s="32">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -1235,10 +1433,22 @@
       <c r="C15" s="12">
         <v>0.9</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="24"/>
+      <c r="D15" s="19">
+        <v>4.8</v>
+      </c>
+      <c r="E15" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="F15" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G15" s="32">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="H15" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
@@ -1250,10 +1460,22 @@
       <c r="C16" s="12">
         <v>0</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="24"/>
+      <c r="D16" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="29">
+        <v>0</v>
+      </c>
+      <c r="F16" s="27">
+        <v>0</v>
+      </c>
+      <c r="G16" s="32" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
@@ -1265,10 +1487,22 @@
       <c r="C17" s="12">
         <v>0.9</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="24"/>
+      <c r="D17" s="19">
+        <v>6</v>
+      </c>
+      <c r="E17" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="F17" s="27">
+        <v>0</v>
+      </c>
+      <c r="G17" s="32">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="H17" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -1280,10 +1514,22 @@
       <c r="C18" s="12">
         <v>0.3</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="24"/>
+      <c r="D18" s="19">
+        <v>4.2</v>
+      </c>
+      <c r="E18" s="29">
+        <v>0</v>
+      </c>
+      <c r="F18" s="27">
+        <v>0</v>
+      </c>
+      <c r="G18" s="32">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
@@ -1295,10 +1541,22 @@
       <c r="C19" s="12">
         <v>0.4</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="24"/>
+      <c r="D19" s="19">
+        <v>3</v>
+      </c>
+      <c r="E19" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="F19" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G19" s="32">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H19" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
@@ -1310,10 +1568,22 @@
       <c r="C20" s="12">
         <v>0.8</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="24"/>
+      <c r="D20" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="29">
+        <v>0</v>
+      </c>
+      <c r="F20" s="27">
+        <v>0</v>
+      </c>
+      <c r="G20" s="32" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
@@ -1325,10 +1595,22 @@
       <c r="C21" s="12">
         <v>0</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="24"/>
+      <c r="D21" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="29">
+        <v>0</v>
+      </c>
+      <c r="F21" s="27">
+        <v>0</v>
+      </c>
+      <c r="G21" s="32" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
@@ -1340,10 +1622,25 @@
       <c r="C22" s="12">
         <v>0.5</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="24"/>
+      <c r="D22" s="19">
+        <v>3.6</v>
+      </c>
+      <c r="E22" s="19">
+        <v>2</v>
+      </c>
+      <c r="F22" s="27">
+        <v>0.7</v>
+      </c>
+      <c r="G22" s="32">
+        <f t="shared" si="0"/>
+        <v>6.3</v>
+      </c>
+      <c r="H22" s="1">
+        <v>12</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
@@ -1355,10 +1652,22 @@
       <c r="C23" s="12">
         <v>0</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="24"/>
+      <c r="D23" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="29">
+        <v>0</v>
+      </c>
+      <c r="F23" s="27">
+        <v>0</v>
+      </c>
+      <c r="G23" s="32" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
@@ -1370,10 +1679,25 @@
       <c r="C24" s="12">
         <v>0.5</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="24"/>
+      <c r="D24" s="19">
+        <v>5.4</v>
+      </c>
+      <c r="E24" s="19">
+        <v>1.8</v>
+      </c>
+      <c r="F24" s="27">
+        <v>0</v>
+      </c>
+      <c r="G24" s="32">
+        <f t="shared" si="0"/>
+        <v>7.2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>11</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
@@ -1385,10 +1709,22 @@
       <c r="C25" s="12">
         <v>0.9</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="24"/>
+      <c r="D25" s="19">
+        <v>6</v>
+      </c>
+      <c r="E25" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="F25" s="27">
+        <v>0</v>
+      </c>
+      <c r="G25" s="32">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="H25" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
@@ -1400,10 +1736,22 @@
       <c r="C26" s="12">
         <v>0.9</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="24"/>
+      <c r="D26" s="19">
+        <v>6</v>
+      </c>
+      <c r="E26" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="F26" s="27">
+        <v>0</v>
+      </c>
+      <c r="G26" s="32">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="H26" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
@@ -1415,10 +1763,22 @@
       <c r="C27" s="12">
         <v>0.9</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="24"/>
+      <c r="D27" s="19">
+        <v>6</v>
+      </c>
+      <c r="E27" s="19">
+        <v>2</v>
+      </c>
+      <c r="F27" s="27">
+        <v>0</v>
+      </c>
+      <c r="G27" s="32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H27" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
@@ -1430,10 +1790,25 @@
       <c r="C28" s="12">
         <v>1</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="24"/>
+      <c r="D28" s="19">
+        <v>6</v>
+      </c>
+      <c r="E28" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="F28" s="27">
+        <v>0</v>
+      </c>
+      <c r="G28" s="32">
+        <f t="shared" si="0"/>
+        <v>7.9</v>
+      </c>
+      <c r="H28" s="1">
+        <v>9</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
@@ -1445,10 +1820,22 @@
       <c r="C29" s="12">
         <v>1</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="24"/>
+      <c r="D29" s="19">
+        <v>6</v>
+      </c>
+      <c r="E29" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="F29" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G29" s="32">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+      <c r="H29" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
@@ -1460,15 +1847,24 @@
       <c r="C30" s="12">
         <v>0.6</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="24"/>
+      <c r="D30" s="19">
+        <v>5.4</v>
+      </c>
+      <c r="E30" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F30" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G30" s="32">
+        <f t="shared" si="0"/>
+        <v>9.1000000000000014</v>
+      </c>
       <c r="H30" s="1">
         <v>5</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1481,10 +1877,22 @@
       <c r="C31" s="12">
         <v>0.6</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="24"/>
+      <c r="D31" s="19">
+        <v>6</v>
+      </c>
+      <c r="E31" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="F31" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G31" s="32">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H31" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
@@ -1496,10 +1904,22 @@
       <c r="C32" s="12">
         <v>0.4</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="24"/>
+      <c r="D32" s="19">
+        <v>4.8</v>
+      </c>
+      <c r="E32" s="29">
+        <v>0</v>
+      </c>
+      <c r="F32" s="27">
+        <v>0</v>
+      </c>
+      <c r="G32" s="32">
+        <f t="shared" si="0"/>
+        <v>4.8</v>
+      </c>
+      <c r="H32" s="30" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
@@ -1511,12 +1931,24 @@
       <c r="C33" s="12">
         <v>0.8</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="24"/>
+      <c r="D33" s="19">
+        <v>6</v>
+      </c>
+      <c r="E33" s="29">
+        <v>0</v>
+      </c>
+      <c r="F33" s="27">
+        <v>0</v>
+      </c>
+      <c r="G33" s="32">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H33" s="30" t="s">
+        <v>101</v>
+      </c>
       <c r="I33" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1529,10 +1961,22 @@
       <c r="C34" s="12">
         <v>0.3</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="24"/>
+      <c r="D34" s="19">
+        <v>4.8</v>
+      </c>
+      <c r="E34" s="29">
+        <v>0</v>
+      </c>
+      <c r="F34" s="27">
+        <v>0</v>
+      </c>
+      <c r="G34" s="32">
+        <f t="shared" si="0"/>
+        <v>4.8</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
@@ -1544,10 +1988,25 @@
       <c r="C35" s="12">
         <v>1</v>
       </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="24"/>
+      <c r="D35" s="19">
+        <v>6</v>
+      </c>
+      <c r="E35" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="F35" s="20">
+        <v>0.7</v>
+      </c>
+      <c r="G35" s="32">
+        <f t="shared" si="0"/>
+        <v>8.6</v>
+      </c>
+      <c r="H35" s="1">
+        <v>9</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
@@ -1559,10 +2018,22 @@
       <c r="C36" s="12">
         <v>0</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="24"/>
+      <c r="D36" s="19">
+        <v>6</v>
+      </c>
+      <c r="E36" s="19">
+        <v>2</v>
+      </c>
+      <c r="F36" s="27">
+        <v>0</v>
+      </c>
+      <c r="G36" s="32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H36" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
@@ -1574,10 +2045,22 @@
       <c r="C37" s="12">
         <v>0.8</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="24"/>
+      <c r="D37" s="19">
+        <v>6</v>
+      </c>
+      <c r="E37" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="F37" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G37" s="32">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H37" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
@@ -1589,12 +2072,24 @@
       <c r="C38" s="12">
         <v>0</v>
       </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="24"/>
+      <c r="D38" s="19">
+        <v>6</v>
+      </c>
+      <c r="E38" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="F38" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G38" s="32">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="H38" s="1">
         <v>6</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -1607,10 +2102,22 @@
       <c r="C39" s="12">
         <v>0.9</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="24"/>
+      <c r="D39" s="19">
+        <v>5.4</v>
+      </c>
+      <c r="E39" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="F39" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G39" s="32">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+      <c r="H39" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
@@ -1622,10 +2129,25 @@
       <c r="C40" s="12">
         <v>1</v>
       </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="24"/>
+      <c r="D40" s="19">
+        <v>6</v>
+      </c>
+      <c r="E40" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="F40" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G40" s="32">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+      <c r="H40" s="1">
+        <v>9</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
@@ -1637,25 +2159,55 @@
       <c r="C41" s="12">
         <v>0.8</v>
       </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="24"/>
+      <c r="D41" s="19">
+        <v>5.4</v>
+      </c>
+      <c r="E41" s="19">
+        <v>1.9</v>
+      </c>
+      <c r="F41" s="27">
+        <v>0</v>
+      </c>
+      <c r="G41" s="32">
+        <f t="shared" si="0"/>
+        <v>7.3000000000000007</v>
+      </c>
+      <c r="H41" s="1">
+        <v>9</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="42" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="23" t="s">
         <v>33</v>
       </c>
       <c r="C42" s="13">
         <v>0.3</v>
       </c>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="28"/>
+      <c r="D42" s="24">
+        <v>6</v>
+      </c>
+      <c r="E42" s="24">
+        <v>1.9</v>
+      </c>
+      <c r="F42" s="28">
+        <v>0</v>
+      </c>
+      <c r="G42" s="33">
+        <f>D42+E42+F42</f>
+        <v>7.9</v>
+      </c>
+      <c r="H42" s="1">
+        <v>9</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B44" s="16" t="s">
@@ -1671,8 +2223,12 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" display="https://github.com/Ar1an3/GerTarefa" xr:uid="{3CC27A7A-E5AC-4FE0-879D-E1267B5AFB88}"/>
+    <hyperlink ref="I10" r:id="rId2" display="https://github.com/deivomaciel/Trabalho-Eng.-de-Software" xr:uid="{C8C18BE7-2F9D-46A6-B928-ED0A5751304D}"/>
+    <hyperlink ref="I40" r:id="rId3" xr:uid="{87B74BB7-B277-413F-B3C2-E8F1F4192237}"/>
+    <hyperlink ref="I3" r:id="rId4" xr:uid="{7F4E1BB5-3714-445C-ADBB-59DB8243E626}"/>
+    <hyperlink ref="I24" r:id="rId5" display="https://github.com/Germinio-marcelo/Engenharia-de-software-hugo.." xr:uid="{878810AB-F544-4A01-9924-E9C00FF5F97C}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>